<commit_message>
Direction control loop changed Max speed now 76%
</commit_message>
<xml_diff>
--- a/Simulate/Speed vs angle tabel.xlsx
+++ b/Simulate/Speed vs angle tabel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\NicE-Buoy\Simulate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1ED229B-C9C4-42F5-BFF8-2F28A537D7C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32E5FEB-E67B-4915-BC4A-2F9429BDE381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{428E957F-06F8-4CEF-BF3C-B02B99AED834}"/>
+    <workbookView xWindow="-22530" yWindow="2220" windowWidth="21600" windowHeight="11235" xr2:uid="{428E957F-06F8-4CEF-BF3C-B02B99AED834}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Error</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Speed*(1-SIN(error)*-1)</t>
+  </si>
+  <si>
+    <t>tan(error)</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -109,6 +112,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,23 +430,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8E8A795-9140-4AC7-81D7-8514ABB944E0}">
-  <dimension ref="B2:I41"/>
+  <dimension ref="B2:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="9.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="36" style="4" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="4" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="47.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="2" customWidth="1"/>
+    <col min="10" max="10" width="29.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -453,398 +459,808 @@
       <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <f>COS(C3*PI()/180)</f>
+        <f>COS($C$3*PI()/180)</f>
         <v>1</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E24" si="0">SIN(C3*PI()/180)</f>
+        <f t="shared" ref="E3:F11" si="0">SIN(C3*PI()/180)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="3">
-        <f>B3*D3*(1-E3)</f>
-        <v>10</v>
-      </c>
-      <c r="G3" s="5">
-        <f>B3*D3*(1-E3*-1)</f>
-        <v>10</v>
-      </c>
-      <c r="H3" s="3">
-        <f>B3*(1-E3)</f>
-        <v>10</v>
-      </c>
-      <c r="I3" s="5">
-        <f>B3*(1-E3*-1)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <f>$B$3*TAN(C3*PI()/180)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <f>$B$3*D3*(1-E3)</f>
+        <v>76</v>
+      </c>
+      <c r="H3" s="5">
+        <f>$B$3*D3*(1-E3*-1)</f>
+        <v>76</v>
+      </c>
+      <c r="I3" s="3">
+        <f>$B$3*(1-E3)</f>
+        <v>76</v>
+      </c>
+      <c r="J3" s="5">
+        <f>$B$3*(1-E3*-1)</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <f>COS(C4*PI()/180)</f>
+        <f t="shared" ref="D4:D8" si="1">COS(C4*PI()/180)</f>
         <v>0.98480775301220802</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>0.17364817766693033</v>
       </c>
-      <c r="F4" s="3">
-        <f>B3*D4*(1-E4)</f>
-        <v>8.1379768134937365</v>
-      </c>
-      <c r="G4" s="5">
-        <f>B3*D4*(1-E4*-1)</f>
-        <v>11.558178246750423</v>
-      </c>
-      <c r="H4" s="3">
-        <f>B3*(1-E4)</f>
-        <v>8.2635182233306974</v>
-      </c>
-      <c r="I4" s="5">
-        <f>B3*(1-E4*-1)</f>
-        <v>11.736481776669303</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F34" si="2">$B$3*TAN(C4*PI()/180)</f>
+        <v>13.400850533843338</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" ref="G4:G34" si="3">$B$3*D4*(1-E4)</f>
+        <v>61.848623782552409</v>
+      </c>
+      <c r="H4" s="5">
+        <f t="shared" ref="H4:H34" si="4">$B$3*D4*(1-E4*-1)</f>
+        <v>87.84215467530322</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I34" si="5">$B$3*(1-E4)</f>
+        <v>62.8027384973133</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" ref="J4:J34" si="6">$B$3*(1-E4*-1)</f>
+        <v>89.1972615026867</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>20</v>
       </c>
       <c r="D5" s="1">
-        <f>COS(C5*PI()/180)</f>
+        <f t="shared" si="1"/>
         <v>0.93969262078590843</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>0.34202014332566871</v>
       </c>
-      <c r="F5" s="3">
-        <f>B3*D5*(1-E5)</f>
-        <v>6.1829881594263885</v>
-      </c>
-      <c r="G5" s="5">
-        <f>B3*D5*(1-E5*-1)</f>
-        <v>12.610864256291782</v>
-      </c>
-      <c r="H5" s="3">
-        <f>B3*(1-E5)</f>
-        <v>6.5797985667433139</v>
-      </c>
-      <c r="I5" s="5">
-        <f>B3*(1-E5*-1)</f>
-        <v>13.420201433256686</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F5" s="1">
+        <f t="shared" si="2"/>
+        <v>27.661737804231379</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="3"/>
+        <v>46.990710011640552</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="4"/>
+        <v>95.842568347817533</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="5"/>
+        <v>50.006469107249181</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="6"/>
+        <v>101.99353089275081</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>30</v>
       </c>
       <c r="D6" s="1">
-        <f>COS(C6*PI()/180)</f>
+        <f t="shared" si="1"/>
         <v>0.86602540378443871</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>0.49999999999999994</v>
       </c>
-      <c r="F6" s="3">
-        <f>B3*D6*(1-E6)</f>
-        <v>4.3301270189221936</v>
-      </c>
-      <c r="G6" s="5">
-        <f>B3*D6*(1-E6*-1)</f>
-        <v>12.99038105676658</v>
-      </c>
-      <c r="H6" s="3">
-        <f>B3*(1-E6)</f>
-        <v>5</v>
-      </c>
-      <c r="I6" s="5">
-        <f>B3*(1-E6*-1)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F6" s="1">
+        <f t="shared" si="2"/>
+        <v>43.878620458411554</v>
+      </c>
+      <c r="G6" s="3">
+        <f t="shared" si="3"/>
+        <v>32.908965343808674</v>
+      </c>
+      <c r="H6" s="5">
+        <f t="shared" si="4"/>
+        <v>98.726896031426023</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="6"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>40</v>
       </c>
       <c r="D7" s="1">
-        <f>COS(C7*PI()/180)</f>
+        <f t="shared" si="1"/>
         <v>0.76604444311897801</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>0.64278760968653925</v>
       </c>
-      <c r="F7" s="3">
-        <f>B3*D7*(1-E7)</f>
-        <v>2.7364056661287406</v>
-      </c>
-      <c r="G7" s="5">
-        <f>B3*D7*(1-E7*-1)</f>
-        <v>12.584483196250819</v>
-      </c>
-      <c r="H7" s="3">
-        <f>B3*(1-E7)</f>
-        <v>3.5721239031346075</v>
-      </c>
-      <c r="I7" s="5">
-        <f>B3*(1-E7*-1)</f>
-        <v>16.427876096865393</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F7" s="1">
+        <f t="shared" si="2"/>
+        <v>63.771571969473271</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="3"/>
+        <v>20.796683062578428</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="4"/>
+        <v>95.642072291506238</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="5"/>
+        <v>27.148141663823019</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="6"/>
+        <v>124.85185833617699</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>50</v>
       </c>
       <c r="D8" s="1">
-        <f>COS(C8*PI()/180)</f>
+        <f t="shared" si="1"/>
         <v>0.64278760968653936</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>0.76604444311897801</v>
       </c>
-      <c r="F8" s="3">
-        <f>B3*D8*(1-E8)</f>
-        <v>1.5038373318043532</v>
-      </c>
-      <c r="G8" s="5">
-        <f>B3*D8*(1-E8*-1)</f>
-        <v>11.351914861926433</v>
-      </c>
-      <c r="H8" s="3">
-        <f>B3*(1-E8)</f>
-        <v>2.3395555688102201</v>
-      </c>
-      <c r="I8" s="5">
-        <f>B3*(1-E8*-1)</f>
-        <v>17.660444431189781</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F8" s="1">
+        <f t="shared" si="2"/>
+        <v>90.573273037159964</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="3"/>
+        <v>11.429163721713083</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="4"/>
+        <v>86.274552950640881</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="5"/>
+        <v>17.780622322957672</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="6"/>
+        <v>134.21937767704233</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>60</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" ref="D9:D41" si="1">COS(C9*PI()/180)</f>
+        <f t="shared" ref="D9:D12" si="7">COS(C9*PI()/180)</f>
         <v>0.50000000000000011</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>0.8660254037844386</v>
       </c>
-      <c r="F9" s="3">
-        <f>B3*D9*(1-E9)</f>
-        <v>0.66987298107780713</v>
-      </c>
-      <c r="G9" s="5">
-        <f>B3*D9*(1-E9*-1)</f>
-        <v>9.3301270189221945</v>
-      </c>
-      <c r="H9" s="3">
-        <f>B3*(1-E9)</f>
-        <v>1.339745962155614</v>
-      </c>
-      <c r="I9" s="5">
-        <f>B3*(1-E9*-1)</f>
-        <v>18.660254037844386</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F9" s="1">
+        <f t="shared" si="2"/>
+        <v>131.63586137523464</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="3"/>
+        <v>5.0910346561913347</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="4"/>
+        <v>70.908965343808674</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="5"/>
+        <v>10.182069312382666</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="6"/>
+        <v>141.81793068761732</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>70</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.34202014332566882</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>0.93969262078590832</v>
       </c>
-      <c r="F10" s="3">
-        <f>B3*D10*(1-E10)</f>
-        <v>0.20626338482399098</v>
-      </c>
-      <c r="G10" s="5">
-        <f>B3*D10*(1-E10*-1)</f>
-        <v>6.6341394816893864</v>
-      </c>
-      <c r="H10" s="3">
-        <f>B3*(1-E10)</f>
-        <v>0.60307379214091683</v>
-      </c>
-      <c r="I10" s="5">
-        <f>B3*(1-E10*-1)</f>
-        <v>19.396926207859085</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F10" s="1">
+        <f t="shared" si="2"/>
+        <v>208.80828387855124</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="3"/>
+        <v>1.5676017246623315</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="4"/>
+        <v>50.419460060839327</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="5"/>
+        <v>4.5833608202709684</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="6"/>
+        <v>147.41663917972903</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>80</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>0.17364817766693041</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>0.98480775301220802</v>
       </c>
-      <c r="F11" s="3">
-        <f>B3*D11*(1-E11)</f>
-        <v>2.63810600409599E-2</v>
-      </c>
-      <c r="G11" s="5">
-        <f>B3*D11*(1-E11*-1)</f>
-        <v>3.4465824932976488</v>
-      </c>
-      <c r="H11" s="3">
-        <f>B3*(1-E11)</f>
-        <v>0.1519224698779198</v>
-      </c>
-      <c r="I11" s="5">
-        <f>B3*(1-E11*-1)</f>
-        <v>19.848077530122083</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="F11" s="1">
+        <f t="shared" si="2"/>
+        <v>431.01741829094573</v>
+      </c>
+      <c r="G11" s="3">
+        <f t="shared" si="3"/>
+        <v>0.20049605631129525</v>
+      </c>
+      <c r="H11" s="5">
+        <f t="shared" si="4"/>
+        <v>26.194026949062128</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="5"/>
+        <v>1.1546107710721905</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="6"/>
+        <v>150.84538922892781</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>90</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="7"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="E12" s="1">
         <f>SIN(C12*PI()/180)</f>
         <v>1</v>
       </c>
-      <c r="F12" s="3">
-        <f>B3*D12*(1-E12)</f>
+      <c r="F12" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2406659730990495E+18</v>
+      </c>
+      <c r="G12" s="3">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G12" s="5">
-        <f>B3*D12*(1-E12*-1)</f>
-        <v>1.22514845490862E-15</v>
-      </c>
-      <c r="H12" s="3">
-        <f>B3*(1-E12)</f>
+      <c r="H12" s="5">
+        <f t="shared" si="4"/>
+        <v>9.3111282573055121E-15</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I12" s="5">
-        <f>B3*(1-E12*-1)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="5">
+        <f t="shared" si="6"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <f t="shared" ref="D14:D23" si="8">COS(C14*PI()/180)</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <f t="shared" ref="E14:E22" si="9">SIN(C14*PI()/180)</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+      <c r="H14" s="5">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="5"/>
+        <v>76</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="6"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>-10</v>
+      </c>
+      <c r="D15" s="1">
+        <f t="shared" si="8"/>
+        <v>0.98480775301220802</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.17364817766693033</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="2"/>
+        <v>-13.400850533843338</v>
+      </c>
+      <c r="G15" s="3">
+        <f t="shared" si="3"/>
+        <v>87.84215467530322</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" si="4"/>
+        <v>61.848623782552409</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="5"/>
+        <v>89.1972615026867</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="6"/>
+        <v>62.8027384973133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>-20</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="8"/>
+        <v>0.93969262078590843</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.34202014332566871</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="2"/>
+        <v>-27.661737804231379</v>
+      </c>
+      <c r="G16" s="3">
+        <f t="shared" si="3"/>
+        <v>95.842568347817533</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="4"/>
+        <v>46.990710011640552</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="5"/>
+        <v>101.99353089275081</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="6"/>
+        <v>50.006469107249181</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>-30</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="8"/>
+        <v>0.86602540378443871</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.49999999999999994</v>
+      </c>
+      <c r="F17" s="1">
+        <f t="shared" si="2"/>
+        <v>-43.878620458411554</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" si="3"/>
+        <v>98.726896031426023</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="4"/>
+        <v>32.908965343808674</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="5"/>
+        <v>114</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="6"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>-40</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="8"/>
+        <v>0.76604444311897801</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.64278760968653925</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="2"/>
+        <v>-63.771571969473271</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" si="3"/>
+        <v>95.642072291506238</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="4"/>
+        <v>20.796683062578428</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="5"/>
+        <v>124.85185833617699</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="6"/>
+        <v>27.148141663823019</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>-50</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="8"/>
+        <v>0.64278760968653936</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.76604444311897801</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="2"/>
+        <v>-90.573273037159964</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="3"/>
+        <v>86.274552950640881</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="4"/>
+        <v>11.429163721713083</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="5"/>
+        <v>134.21937767704233</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="6"/>
+        <v>17.780622322957672</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>-60</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="8"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="2"/>
+        <v>-131.63586137523464</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="3"/>
+        <v>70.908965343808674</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="4"/>
+        <v>5.0910346561913347</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="5"/>
+        <v>141.81793068761732</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" si="6"/>
+        <v>10.182069312382666</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>-70</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="8"/>
+        <v>0.34202014332566882</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.93969262078590832</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="2"/>
+        <v>-208.80828387855124</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="3"/>
+        <v>50.419460060839327</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="4"/>
+        <v>1.5676017246623315</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="5"/>
+        <v>147.41663917972903</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" si="6"/>
+        <v>4.5833608202709684</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>-80</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="8"/>
+        <v>0.17364817766693041</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.98480775301220802</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="2"/>
+        <v>-431.01741829094573</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="3"/>
+        <v>26.194026949062128</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" si="4"/>
+        <v>0.20049605631129525</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="5"/>
+        <v>150.84538922892781</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" si="6"/>
+        <v>1.1546107710721905</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>-90</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="8"/>
+        <v>6.1257422745431001E-17</v>
+      </c>
+      <c r="E23" s="1">
+        <f>SIN(C23*PI()/180)</f>
+        <v>-1</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.2406659730990495E+18</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="3"/>
+        <v>9.3111282573055121E-15</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="5"/>
+        <v>152</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Some calculation functions added (Cource comuter) and start with python real time chard app
</commit_message>
<xml_diff>
--- a/Simulate/Speed vs angle tabel.xlsx
+++ b/Simulate/Speed vs angle tabel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tmp\NicE-Buoy\Simulate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210E8D4E-7E1B-4ECE-9EBA-724A6BD31534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4728FC5-B2F8-4D24-8A41-6416A7BA395A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="6930" windowWidth="29040" windowHeight="15720" xr2:uid="{428E957F-06F8-4CEF-BF3C-B02B99AED834}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{428E957F-06F8-4CEF-BF3C-B02B99AED834}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Error</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>tan(error)</t>
+  </si>
+  <si>
+    <t>wide</t>
+  </si>
+  <si>
+    <t>dist</t>
+  </si>
+  <si>
+    <t>angle</t>
   </si>
 </sst>
 </file>
@@ -427,20 +436,20 @@
   <dimension ref="B2:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.7265625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.54296875" customWidth="1"/>
-    <col min="7" max="7" width="35.453125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="47.1796875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="6.26953125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="47.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" style="4" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -464,7 +473,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -475,8 +484,8 @@
         <f>COS($C$3*PI()/180)</f>
         <v>1</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E11" si="0">SIN(C3*PI()/180)</f>
+      <c r="E3" s="1" t="b">
+        <f>D30=SIN(C3*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="F3" s="1">
@@ -495,267 +504,267 @@
         <v>0</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" ref="J3:J12" si="1">COS(I3*PI()/180)</f>
+        <f t="shared" ref="J3:J12" si="0">COS(I3*PI()/180)</f>
         <v>1</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:K11" si="2">SIN(I3*PI()/180)</f>
+        <f t="shared" ref="K3:K11" si="1">SIN(I3*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" ref="L3:L12" si="3">$B$3*TAN(I3*PI()/180)</f>
+        <f t="shared" ref="L3:L12" si="2">$B$3*TAN(I3*PI()/180)</f>
         <v>0</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M12" si="4">$B$3*J3*(1-K3)</f>
+        <f t="shared" ref="M3:M12" si="3">$B$3*J3*(1-K3)</f>
         <v>1</v>
       </c>
       <c r="N3" s="5">
-        <f t="shared" ref="N3:N12" si="5">$B$3*J3*(1-K3*-1)</f>
+        <f t="shared" ref="N3:N12" si="4">$B$3*J3*(1-K3*-1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D8" si="6">COS(C4*PI()/180)</f>
+        <f t="shared" ref="D4:D8" si="5">COS(C4*PI()/180)</f>
         <v>0.98480775301220802</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E3:E11" si="6">SIN(C4*PI()/180)</f>
         <v>0.17364817766693033</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" ref="F4:F20" si="7">$B$3*TAN(C4*PI()/180)</f>
+        <f>$B$3*TAN(C4*PI()/180)</f>
         <v>0.17632698070846498</v>
       </c>
       <c r="G4" s="3">
-        <f t="shared" ref="G4:G20" si="8">$B$3*D4*(1-E4)</f>
+        <f t="shared" ref="G4:G20" si="7">$B$3*D4*(1-E4)</f>
         <v>0.81379768134937369</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" ref="H4:H20" si="9">$B$3*D4*(1-E4*-1)</f>
+        <f t="shared" ref="H4:H20" si="8">$B$3*D4*(1-E4*-1)</f>
         <v>1.1558178246750423</v>
       </c>
       <c r="I4">
         <v>-10</v>
       </c>
       <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98480775301220802</v>
+      </c>
+      <c r="K4" s="1">
         <f t="shared" si="1"/>
-        <v>0.98480775301220802</v>
-      </c>
-      <c r="K4" s="1">
+        <v>-0.17364817766693033</v>
+      </c>
+      <c r="L4" s="1">
         <f t="shared" si="2"/>
-        <v>-0.17364817766693033</v>
-      </c>
-      <c r="L4" s="1">
+        <v>-0.17632698070846498</v>
+      </c>
+      <c r="M4" s="3">
         <f t="shared" si="3"/>
-        <v>-0.17632698070846498</v>
-      </c>
-      <c r="M4" s="3">
+        <v>1.1558178246750423</v>
+      </c>
+      <c r="N4" s="5">
         <f t="shared" si="4"/>
-        <v>1.1558178246750423</v>
-      </c>
-      <c r="N4" s="5">
-        <f t="shared" si="5"/>
         <v>0.81379768134937369</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>20</v>
       </c>
       <c r="D5" s="1">
+        <f t="shared" si="5"/>
+        <v>0.93969262078590843</v>
+      </c>
+      <c r="E5" s="1">
         <f t="shared" si="6"/>
-        <v>0.93969262078590843</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
         <v>0.34202014332566871</v>
       </c>
       <c r="F5" s="1">
+        <f t="shared" ref="F4:F20" si="9">$B$3*TAN(C5*PI()/180)</f>
+        <v>0.36397023426620234</v>
+      </c>
+      <c r="G5" s="3">
         <f t="shared" si="7"/>
-        <v>0.36397023426620234</v>
-      </c>
-      <c r="G5" s="3">
+        <v>0.6182988159426388</v>
+      </c>
+      <c r="H5" s="5">
         <f t="shared" si="8"/>
-        <v>0.6182988159426388</v>
-      </c>
-      <c r="H5" s="5">
-        <f t="shared" si="9"/>
         <v>1.2610864256291781</v>
       </c>
       <c r="I5">
         <v>-20</v>
       </c>
       <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.93969262078590843</v>
+      </c>
+      <c r="K5" s="1">
         <f t="shared" si="1"/>
-        <v>0.93969262078590843</v>
-      </c>
-      <c r="K5" s="1">
+        <v>-0.34202014332566871</v>
+      </c>
+      <c r="L5" s="1">
         <f t="shared" si="2"/>
-        <v>-0.34202014332566871</v>
-      </c>
-      <c r="L5" s="1">
+        <v>-0.36397023426620234</v>
+      </c>
+      <c r="M5" s="3">
         <f t="shared" si="3"/>
-        <v>-0.36397023426620234</v>
-      </c>
-      <c r="M5" s="3">
+        <v>1.2610864256291781</v>
+      </c>
+      <c r="N5" s="5">
         <f t="shared" si="4"/>
-        <v>1.2610864256291781</v>
-      </c>
-      <c r="N5" s="5">
-        <f t="shared" si="5"/>
         <v>0.6182988159426388</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>30</v>
       </c>
       <c r="D6" s="1">
+        <f t="shared" si="5"/>
+        <v>0.86602540378443871</v>
+      </c>
+      <c r="E6" s="1">
         <f t="shared" si="6"/>
-        <v>0.86602540378443871</v>
-      </c>
-      <c r="E6" s="1">
-        <f t="shared" si="0"/>
         <v>0.49999999999999994</v>
       </c>
       <c r="F6" s="1">
+        <f t="shared" si="9"/>
+        <v>0.57735026918962573</v>
+      </c>
+      <c r="G6" s="3">
         <f t="shared" si="7"/>
-        <v>0.57735026918962573</v>
-      </c>
-      <c r="G6" s="3">
+        <v>0.43301270189221935</v>
+      </c>
+      <c r="H6" s="5">
         <f t="shared" si="8"/>
-        <v>0.43301270189221935</v>
-      </c>
-      <c r="H6" s="5">
-        <f t="shared" si="9"/>
         <v>1.299038105676658</v>
       </c>
       <c r="I6">
         <v>-30</v>
       </c>
       <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.86602540378443871</v>
+      </c>
+      <c r="K6" s="1">
         <f t="shared" si="1"/>
-        <v>0.86602540378443871</v>
-      </c>
-      <c r="K6" s="1">
+        <v>-0.49999999999999994</v>
+      </c>
+      <c r="L6" s="1">
         <f t="shared" si="2"/>
-        <v>-0.49999999999999994</v>
-      </c>
-      <c r="L6" s="1">
+        <v>-0.57735026918962573</v>
+      </c>
+      <c r="M6" s="3">
         <f t="shared" si="3"/>
-        <v>-0.57735026918962573</v>
-      </c>
-      <c r="M6" s="3">
+        <v>1.299038105676658</v>
+      </c>
+      <c r="N6" s="5">
         <f t="shared" si="4"/>
-        <v>1.299038105676658</v>
-      </c>
-      <c r="N6" s="5">
-        <f t="shared" si="5"/>
         <v>0.43301270189221935</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>40</v>
       </c>
       <c r="D7" s="1">
+        <f t="shared" si="5"/>
+        <v>0.76604444311897801</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="6"/>
+        <v>0.64278760968653925</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="9"/>
+        <v>0.83909963117727993</v>
+      </c>
+      <c r="G7" s="3">
+        <f t="shared" si="7"/>
+        <v>0.27364056661287406</v>
+      </c>
+      <c r="H7" s="5">
+        <f t="shared" si="8"/>
+        <v>1.258448319625082</v>
+      </c>
+      <c r="I7">
+        <v>-40</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76604444311897801</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.64278760968653925</v>
+      </c>
+      <c r="L7" s="1">
+        <f t="shared" si="2"/>
+        <v>-0.83909963117727993</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="3"/>
+        <v>1.258448319625082</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="4"/>
+        <v>0.27364056661287406</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="5"/>
+        <v>0.64278760968653936</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="6"/>
         <v>0.76604444311897801</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.64278760968653925</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
+        <f t="shared" si="9"/>
+        <v>1.19175359259421</v>
+      </c>
+      <c r="G8" s="3">
         <f t="shared" si="7"/>
-        <v>0.83909963117727993</v>
-      </c>
-      <c r="G7" s="3">
+        <v>0.15038373318043533</v>
+      </c>
+      <c r="H8" s="5">
         <f t="shared" si="8"/>
-        <v>0.27364056661287406</v>
-      </c>
-      <c r="H7" s="5">
-        <f t="shared" si="9"/>
-        <v>1.258448319625082</v>
-      </c>
-      <c r="I7">
-        <v>-40</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="1"/>
-        <v>0.76604444311897801</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="2"/>
-        <v>-0.64278760968653925</v>
-      </c>
-      <c r="L7" s="1">
-        <f t="shared" si="3"/>
-        <v>-0.83909963117727993</v>
-      </c>
-      <c r="M7" s="3">
-        <f t="shared" si="4"/>
-        <v>1.258448319625082</v>
-      </c>
-      <c r="N7" s="5">
-        <f t="shared" si="5"/>
-        <v>0.27364056661287406</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
-      <c r="C8">
-        <v>50</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="6"/>
-        <v>0.64278760968653936</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="0"/>
-        <v>0.76604444311897801</v>
-      </c>
-      <c r="F8" s="1">
-        <f t="shared" si="7"/>
-        <v>1.19175359259421</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="8"/>
-        <v>0.15038373318043533</v>
-      </c>
-      <c r="H8" s="5">
-        <f t="shared" si="9"/>
         <v>1.1351914861926433</v>
       </c>
       <c r="I8">
         <v>-50</v>
       </c>
       <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.64278760968653936</v>
+      </c>
+      <c r="K8" s="1">
         <f t="shared" si="1"/>
-        <v>0.64278760968653936</v>
-      </c>
-      <c r="K8" s="1">
+        <v>-0.76604444311897801</v>
+      </c>
+      <c r="L8" s="1">
         <f t="shared" si="2"/>
-        <v>-0.76604444311897801</v>
-      </c>
-      <c r="L8" s="1">
+        <v>-1.19175359259421</v>
+      </c>
+      <c r="M8" s="3">
         <f t="shared" si="3"/>
-        <v>-1.19175359259421</v>
-      </c>
-      <c r="M8" s="3">
+        <v>1.1351914861926433</v>
+      </c>
+      <c r="N8" s="5">
         <f t="shared" si="4"/>
-        <v>1.1351914861926433</v>
-      </c>
-      <c r="N8" s="5">
-        <f t="shared" si="5"/>
         <v>0.15038373318043533</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>60</v>
       </c>
@@ -764,46 +773,46 @@
         <v>0.50000000000000011</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.8660254037844386</v>
       </c>
       <c r="F9" s="1">
+        <f t="shared" si="9"/>
+        <v>1.7320508075688767</v>
+      </c>
+      <c r="G9" s="3">
         <f t="shared" si="7"/>
-        <v>1.7320508075688767</v>
-      </c>
-      <c r="G9" s="3">
+        <v>6.6987298107780716E-2</v>
+      </c>
+      <c r="H9" s="5">
         <f t="shared" si="8"/>
-        <v>6.6987298107780716E-2</v>
-      </c>
-      <c r="H9" s="5">
-        <f t="shared" si="9"/>
         <v>0.93301270189221952</v>
       </c>
       <c r="I9">
         <v>-60</v>
       </c>
       <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="K9" s="1">
         <f t="shared" si="1"/>
-        <v>0.50000000000000011</v>
-      </c>
-      <c r="K9" s="1">
+        <v>-0.8660254037844386</v>
+      </c>
+      <c r="L9" s="1">
         <f t="shared" si="2"/>
-        <v>-0.8660254037844386</v>
-      </c>
-      <c r="L9" s="1">
+        <v>-1.7320508075688767</v>
+      </c>
+      <c r="M9" s="3">
         <f t="shared" si="3"/>
-        <v>-1.7320508075688767</v>
-      </c>
-      <c r="M9" s="3">
+        <v>0.93301270189221952</v>
+      </c>
+      <c r="N9" s="5">
         <f t="shared" si="4"/>
-        <v>0.93301270189221952</v>
-      </c>
-      <c r="N9" s="5">
-        <f t="shared" si="5"/>
         <v>6.6987298107780716E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>70</v>
       </c>
@@ -812,46 +821,46 @@
         <v>0.34202014332566882</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.93969262078590832</v>
       </c>
       <c r="F10" s="1">
+        <f t="shared" si="9"/>
+        <v>2.7474774194546216</v>
+      </c>
+      <c r="G10" s="3">
         <f t="shared" si="7"/>
-        <v>2.7474774194546216</v>
-      </c>
-      <c r="G10" s="3">
+        <v>2.0626338482399097E-2</v>
+      </c>
+      <c r="H10" s="5">
         <f t="shared" si="8"/>
-        <v>2.0626338482399097E-2</v>
-      </c>
-      <c r="H10" s="5">
-        <f t="shared" si="9"/>
         <v>0.66341394816893862</v>
       </c>
       <c r="I10">
         <v>-70</v>
       </c>
       <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.34202014332566882</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" si="1"/>
-        <v>0.34202014332566882</v>
-      </c>
-      <c r="K10" s="1">
+        <v>-0.93969262078590832</v>
+      </c>
+      <c r="L10" s="1">
         <f t="shared" si="2"/>
-        <v>-0.93969262078590832</v>
-      </c>
-      <c r="L10" s="1">
+        <v>-2.7474774194546216</v>
+      </c>
+      <c r="M10" s="3">
         <f t="shared" si="3"/>
-        <v>-2.7474774194546216</v>
-      </c>
-      <c r="M10" s="3">
+        <v>0.66341394816893862</v>
+      </c>
+      <c r="N10" s="5">
         <f t="shared" si="4"/>
-        <v>0.66341394816893862</v>
-      </c>
-      <c r="N10" s="5">
-        <f t="shared" si="5"/>
         <v>2.0626338482399097E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>80</v>
       </c>
@@ -860,46 +869,46 @@
         <v>0.17364817766693041</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>0.98480775301220802</v>
       </c>
       <c r="F11" s="1">
+        <f t="shared" si="9"/>
+        <v>5.6712818196177066</v>
+      </c>
+      <c r="G11" s="3">
         <f t="shared" si="7"/>
-        <v>5.6712818196177066</v>
-      </c>
-      <c r="G11" s="3">
+        <v>2.6381060040959899E-3</v>
+      </c>
+      <c r="H11" s="5">
         <f t="shared" si="8"/>
-        <v>2.6381060040959899E-3</v>
-      </c>
-      <c r="H11" s="5">
-        <f t="shared" si="9"/>
         <v>0.34465824932976485</v>
       </c>
       <c r="I11">
         <v>-80</v>
       </c>
       <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.17364817766693041</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="1"/>
-        <v>0.17364817766693041</v>
-      </c>
-      <c r="K11" s="1">
+        <v>-0.98480775301220802</v>
+      </c>
+      <c r="L11" s="1">
         <f t="shared" si="2"/>
-        <v>-0.98480775301220802</v>
-      </c>
-      <c r="L11" s="1">
+        <v>-5.6712818196177066</v>
+      </c>
+      <c r="M11" s="3">
         <f t="shared" si="3"/>
-        <v>-5.6712818196177066</v>
-      </c>
-      <c r="M11" s="3">
+        <v>0.34465824932976485</v>
+      </c>
+      <c r="N11" s="5">
         <f t="shared" si="4"/>
-        <v>0.34465824932976485</v>
-      </c>
-      <c r="N11" s="5">
-        <f t="shared" si="5"/>
         <v>2.6381060040959899E-3</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>90</v>
       </c>
@@ -912,22 +921,22 @@
         <v>1</v>
       </c>
       <c r="F12" s="1">
+        <f t="shared" si="9"/>
+        <v>1.6324552277619072E+16</v>
+      </c>
+      <c r="G12" s="3">
         <f t="shared" si="7"/>
-        <v>1.6324552277619072E+16</v>
-      </c>
-      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="5">
-        <f t="shared" si="9"/>
         <v>1.22514845490862E-16</v>
       </c>
       <c r="I12">
         <v>-90</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.1257422745431001E-17</v>
       </c>
       <c r="K12" s="1">
@@ -935,19 +944,19 @@
         <v>-1</v>
       </c>
       <c r="L12" s="1">
+        <f t="shared" si="2"/>
+        <v>-1.6324552277619072E+16</v>
+      </c>
+      <c r="M12" s="3">
         <f t="shared" si="3"/>
-        <v>-1.6324552277619072E+16</v>
-      </c>
-      <c r="M12" s="3">
+        <v>1.22514845490862E-16</v>
+      </c>
+      <c r="N12" s="5">
         <f t="shared" si="4"/>
-        <v>1.22514845490862E-16</v>
-      </c>
-      <c r="N12" s="5">
-        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>100</v>
       </c>
@@ -960,15 +969,15 @@
         <v>0.98480775301220802</v>
       </c>
       <c r="F13" s="1">
+        <f t="shared" si="9"/>
+        <v>-5.6712818196177111</v>
+      </c>
+      <c r="G13" s="3">
         <f t="shared" si="7"/>
-        <v>-5.6712818196177111</v>
-      </c>
-      <c r="G13" s="3">
+        <v>-2.6381060040959886E-3</v>
+      </c>
+      <c r="H13" s="5">
         <f t="shared" si="8"/>
-        <v>-2.6381060040959886E-3</v>
-      </c>
-      <c r="H13" s="5">
-        <f t="shared" si="9"/>
         <v>-0.34465824932976463</v>
       </c>
       <c r="I13">
@@ -995,7 +1004,7 @@
         <v>-2.6381060040959886E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>110</v>
       </c>
@@ -1008,15 +1017,15 @@
         <v>0.93969262078590843</v>
       </c>
       <c r="F14" s="1">
+        <f t="shared" si="9"/>
+        <v>-2.7474774194546225</v>
+      </c>
+      <c r="G14" s="3">
         <f t="shared" si="7"/>
-        <v>-2.7474774194546225</v>
-      </c>
-      <c r="G14" s="3">
+        <v>-2.0626338482399052E-2</v>
+      </c>
+      <c r="H14" s="5">
         <f t="shared" si="8"/>
-        <v>-2.0626338482399052E-2</v>
-      </c>
-      <c r="H14" s="5">
-        <f t="shared" si="9"/>
         <v>-0.66341394816893839</v>
       </c>
       <c r="I14">
@@ -1043,7 +1052,7 @@
         <v>-2.0626338482399052E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>120</v>
       </c>
@@ -1056,15 +1065,15 @@
         <v>0.86602540378443871</v>
       </c>
       <c r="F15" s="1">
+        <f t="shared" si="9"/>
+        <v>-1.7320508075688783</v>
+      </c>
+      <c r="G15" s="3">
         <f t="shared" si="7"/>
-        <v>-1.7320508075688783</v>
-      </c>
-      <c r="G15" s="3">
+        <v>-6.6987298107780618E-2</v>
+      </c>
+      <c r="H15" s="5">
         <f t="shared" si="8"/>
-        <v>-6.6987298107780618E-2</v>
-      </c>
-      <c r="H15" s="5">
-        <f t="shared" si="9"/>
         <v>-0.93301270189221897</v>
       </c>
       <c r="I15">
@@ -1091,7 +1100,7 @@
         <v>-6.6987298107780618E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>130</v>
       </c>
@@ -1104,15 +1113,15 @@
         <v>0.76604444311897801</v>
       </c>
       <c r="F16" s="1">
+        <f t="shared" si="9"/>
+        <v>-1.19175359259421</v>
+      </c>
+      <c r="G16" s="3">
         <f t="shared" si="7"/>
-        <v>-1.19175359259421</v>
-      </c>
-      <c r="G16" s="3">
+        <v>-0.15038373318043533</v>
+      </c>
+      <c r="H16" s="5">
         <f t="shared" si="8"/>
-        <v>-0.15038373318043533</v>
-      </c>
-      <c r="H16" s="5">
-        <f t="shared" si="9"/>
         <v>-1.1351914861926433</v>
       </c>
       <c r="I16">
@@ -1139,7 +1148,7 @@
         <v>-0.15038373318043533</v>
       </c>
     </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>140</v>
       </c>
@@ -1152,15 +1161,15 @@
         <v>0.64278760968653947</v>
       </c>
       <c r="F17" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.83909963117728037</v>
+      </c>
+      <c r="G17" s="3">
         <f t="shared" si="7"/>
-        <v>-0.83909963117728037</v>
-      </c>
-      <c r="G17" s="3">
+        <v>-0.27364056661287384</v>
+      </c>
+      <c r="H17" s="5">
         <f t="shared" si="8"/>
-        <v>-0.27364056661287384</v>
-      </c>
-      <c r="H17" s="5">
-        <f t="shared" si="9"/>
         <v>-1.258448319625082</v>
       </c>
       <c r="I17">
@@ -1187,7 +1196,7 @@
         <v>-0.27364056661287384</v>
       </c>
     </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>150</v>
       </c>
@@ -1200,15 +1209,15 @@
         <v>0.49999999999999994</v>
       </c>
       <c r="F18" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.57735026918962573</v>
+      </c>
+      <c r="G18" s="3">
         <f t="shared" si="7"/>
-        <v>-0.57735026918962573</v>
-      </c>
-      <c r="G18" s="3">
+        <v>-0.43301270189221935</v>
+      </c>
+      <c r="H18" s="5">
         <f t="shared" si="8"/>
-        <v>-0.43301270189221935</v>
-      </c>
-      <c r="H18" s="5">
-        <f t="shared" si="9"/>
         <v>-1.299038105676658</v>
       </c>
       <c r="I18">
@@ -1235,7 +1244,7 @@
         <v>-0.43301270189221935</v>
       </c>
     </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>160</v>
       </c>
@@ -1248,15 +1257,15 @@
         <v>0.34202014332566888</v>
       </c>
       <c r="F19" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.36397023426620256</v>
+      </c>
+      <c r="G19" s="3">
         <f t="shared" si="7"/>
-        <v>-0.36397023426620256</v>
-      </c>
-      <c r="G19" s="3">
+        <v>-0.61829881594263858</v>
+      </c>
+      <c r="H19" s="5">
         <f t="shared" si="8"/>
-        <v>-0.61829881594263858</v>
-      </c>
-      <c r="H19" s="5">
-        <f t="shared" si="9"/>
         <v>-1.2610864256291781</v>
       </c>
       <c r="I19">
@@ -1283,7 +1292,7 @@
         <v>-0.61829881594263858</v>
       </c>
     </row>
-    <row r="20" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>170</v>
       </c>
@@ -1296,15 +1305,15 @@
         <v>0.17364817766693028</v>
       </c>
       <c r="F20" s="1">
+        <f t="shared" si="9"/>
+        <v>-0.17632698070846489</v>
+      </c>
+      <c r="G20" s="3">
         <f t="shared" si="7"/>
-        <v>-0.17632698070846489</v>
-      </c>
-      <c r="G20" s="3">
+        <v>-0.81379768134937369</v>
+      </c>
+      <c r="H20" s="5">
         <f t="shared" si="8"/>
-        <v>-0.81379768134937369</v>
-      </c>
-      <c r="H20" s="5">
-        <f t="shared" si="9"/>
         <v>-1.1558178246750423</v>
       </c>
       <c r="I20">
@@ -1331,7 +1340,7 @@
         <v>-0.81379768134937369</v>
       </c>
     </row>
-    <row r="21" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="3"/>
@@ -1343,7 +1352,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="5"/>
     </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="3"/>
@@ -1355,119 +1364,138 @@
       <c r="M22" s="3"/>
       <c r="N22" s="5"/>
     </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="3"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="3"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="3"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="3"/>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="3"/>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="1">
+        <v>-10</v>
+      </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="3"/>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1">
+        <v>500</v>
+      </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="3"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="1">
+        <f>(ATAN(D28/D29))*180/PI()</f>
+        <v>-1.1457628381751035</v>
+      </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="3"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="3"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="3"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="3"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="3"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C46">
         <v>100</v>
       </c>
@@ -1492,7 +1520,7 @@
         <v>-0.34465824932976463</v>
       </c>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C47">
         <v>110</v>
       </c>
@@ -1517,7 +1545,7 @@
         <v>-0.66341394816893839</v>
       </c>
     </row>
-    <row r="48" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>120</v>
       </c>
@@ -1542,7 +1570,7 @@
         <v>-0.93301270189221897</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49">
         <v>130</v>
       </c>
@@ -1567,7 +1595,7 @@
         <v>-1.1351914861926433</v>
       </c>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50">
         <v>140</v>
       </c>
@@ -1592,7 +1620,7 @@
         <v>-1.258448319625082</v>
       </c>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C51">
         <v>150</v>
       </c>
@@ -1617,7 +1645,7 @@
         <v>-1.299038105676658</v>
       </c>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C52">
         <v>160</v>
       </c>
@@ -1642,7 +1670,7 @@
         <v>-1.2610864256291781</v>
       </c>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C53">
         <v>170</v>
       </c>

</xml_diff>